<commit_message>
removed space before min(utes) and updated German translation
</commit_message>
<xml_diff>
--- a/monitor.translations.xlsx
+++ b/monitor.translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick\git\monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3752BE35-6494-483F-9534-9DCDC546AD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488FE772-EC4E-446C-873C-3BBA664CB40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,9 +189,6 @@
     <t>Batteriepflege</t>
   </si>
   <si>
-    <t>Höchstgeschwindigkeit</t>
-  </si>
-  <si>
     <t>Wartezeit</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>Durchschn. Geschw.</t>
   </si>
   <si>
-    <t>Letzter Lauf</t>
-  </si>
-  <si>
     <t>Gem. snelheid</t>
   </si>
   <si>
@@ -727,6 +721,12 @@
   </si>
   <si>
     <t>Eletrônicos</t>
+  </si>
+  <si>
+    <t>Zuletzt aktualisiert</t>
+  </si>
+  <si>
+    <t>Höchstgeschw.</t>
   </si>
 </sst>
 </file>
@@ -1081,14 +1081,14 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
@@ -1105,7 +1105,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -1211,34 +1211,34 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1252,31 +1252,31 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1290,31 +1290,31 @@
         <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1331,28 +1331,28 @@
         <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1369,10 +1369,10 @@
         <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
         <v>39</v>
@@ -1387,7 +1387,7 @@
         <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L7" t="s">
         <v>39</v>
@@ -1407,16 +1407,16 @@
         <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I8" t="s">
         <v>52</v>
@@ -1425,10 +1425,10 @@
         <v>52</v>
       </c>
       <c r="K8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1436,37 +1436,37 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" t="s">
+        <v>225</v>
+      </c>
+      <c r="F9" t="s">
         <v>226</v>
       </c>
-      <c r="C9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>227</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>228</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>229</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
+        <v>229</v>
+      </c>
+      <c r="K9" t="s">
         <v>230</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>231</v>
-      </c>
-      <c r="J9" t="s">
-        <v>231</v>
-      </c>
-      <c r="K9" t="s">
-        <v>232</v>
-      </c>
-      <c r="L9" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1483,28 +1483,28 @@
         <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1518,31 +1518,31 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1556,31 +1556,31 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J12" t="s">
         <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1591,34 +1591,34 @@
         <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1632,31 +1632,31 @@
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1670,186 +1670,186 @@
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
         <v>68</v>
       </c>
-      <c r="D16" t="s">
-        <v>70</v>
-      </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1857,130 +1857,130 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summary.py: Added translations for standard output and sheetupdate
</commit_message>
<xml_diff>
--- a/monitor.translations.xlsx
+++ b/monitor.translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick\git\monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1576686B-104F-468B-B70F-965486A1BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA08C7A7-18EB-427C-9438-D037B722EE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20445" yWindow="930" windowWidth="17805" windowHeight="18435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="498">
   <si>
     <t>en</t>
   </si>
@@ -714,15 +714,9 @@
     <t>Idle</t>
   </si>
   <si>
-    <t>Gem</t>
-  </si>
-  <si>
     <t>Avg</t>
   </si>
   <si>
-    <t>Batterijonderh</t>
-  </si>
-  <si>
     <t>Batt.Care</t>
   </si>
   <si>
@@ -730,6 +724,801 @@
   </si>
   <si>
     <t>Laatste upd</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>#charges</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>EV range</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>SOC%</t>
+  </si>
+  <si>
+    <t>12V%</t>
+  </si>
+  <si>
+    <t>Periode</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>Adres</t>
+  </si>
+  <si>
+    <t>Vehicle upd</t>
+  </si>
+  <si>
+    <t>GPS update</t>
+  </si>
+  <si>
+    <t>Last entry</t>
+  </si>
+  <si>
+    <t>Last address</t>
+  </si>
+  <si>
+    <t>Driven</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Odometer</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Voertuig upd</t>
+  </si>
+  <si>
+    <t>Laatste regel</t>
+  </si>
+  <si>
+    <t>Laatste adres</t>
+  </si>
+  <si>
+    <t>Gereden</t>
+  </si>
+  <si>
+    <t>#trips</t>
+  </si>
+  <si>
+    <t>#Trips</t>
+  </si>
+  <si>
+    <t>soc perc</t>
+  </si>
+  <si>
+    <t>12volt perc</t>
+  </si>
+  <si>
+    <t>TRIP</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>WEEK</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>TRIPAVG</t>
+  </si>
+  <si>
+    <t>DAYAVG</t>
+  </si>
+  <si>
+    <t>WEEKAVG</t>
+  </si>
+  <si>
+    <t>MONTHAVG</t>
+  </si>
+  <si>
+    <t>YEARLY</t>
+  </si>
+  <si>
+    <t>DAG</t>
+  </si>
+  <si>
+    <t>MAAND</t>
+  </si>
+  <si>
+    <t>JAAR</t>
+  </si>
+  <si>
+    <t>JAARLIJKS</t>
+  </si>
+  <si>
+    <t>Kosten</t>
+  </si>
+  <si>
+    <t>Rit</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>RIT</t>
+  </si>
+  <si>
+    <t>Teller</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Bereik</t>
+  </si>
+  <si>
+    <t>Zeitraum</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Kilometerzähler</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Reichweite</t>
+  </si>
+  <si>
+    <t>Fahrzeugaktualisierung</t>
+  </si>
+  <si>
+    <t>GPS-Update</t>
+  </si>
+  <si>
+    <t>Letzter Eintrag</t>
+  </si>
+  <si>
+    <t>Letzte Adresse</t>
+  </si>
+  <si>
+    <t>Gefahren</t>
+  </si>
+  <si>
+    <t>TAG</t>
+  </si>
+  <si>
+    <t>WOCHE</t>
+  </si>
+  <si>
+    <t>MONAT</t>
+  </si>
+  <si>
+    <t>JAHR</t>
+  </si>
+  <si>
+    <t>JÄHRLICH</t>
+  </si>
+  <si>
+    <t>#Fahrten</t>
+  </si>
+  <si>
+    <t>#Geladen</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>FAHRT</t>
+  </si>
+  <si>
+    <t>#Charging</t>
+  </si>
+  <si>
+    <t>#Opladen</t>
+  </si>
+  <si>
+    <t>#Ritten</t>
+  </si>
+  <si>
+    <t>Période</t>
+  </si>
+  <si>
+    <t>Odomètre</t>
+  </si>
+  <si>
+    <t>Coût</t>
+  </si>
+  <si>
+    <t>COS %</t>
+  </si>
+  <si>
+    <t>Moy</t>
+  </si>
+  <si>
+    <t>#Mise en charge</t>
+  </si>
+  <si>
+    <t>#Voyages</t>
+  </si>
+  <si>
+    <t>Gamme</t>
+  </si>
+  <si>
+    <t>Adresse</t>
+  </si>
+  <si>
+    <t>Mise à jour du véhicule</t>
+  </si>
+  <si>
+    <t>Mise à jour GPS</t>
+  </si>
+  <si>
+    <t>Dernière entrée</t>
+  </si>
+  <si>
+    <t>Dernière adresse</t>
+  </si>
+  <si>
+    <t>Conduit</t>
+  </si>
+  <si>
+    <t>VOYAGE</t>
+  </si>
+  <si>
+    <t>JOURNÉE</t>
+  </si>
+  <si>
+    <t>LA SEMAINE</t>
+  </si>
+  <si>
+    <t>MOIS</t>
+  </si>
+  <si>
+    <t>ANNÉE</t>
+  </si>
+  <si>
+    <t>ANNUEL</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Informazioni</t>
+  </si>
+  <si>
+    <t>Odometro</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>Massimo</t>
+  </si>
+  <si>
+    <t>#Ricarica</t>
+  </si>
+  <si>
+    <t>#Viaggi</t>
+  </si>
+  <si>
+    <t>Allineare</t>
+  </si>
+  <si>
+    <t>Indirizzo</t>
+  </si>
+  <si>
+    <t>Aggiornamento GPS</t>
+  </si>
+  <si>
+    <t>Ultimo ingresso</t>
+  </si>
+  <si>
+    <t>Ultimo indirizzo</t>
+  </si>
+  <si>
+    <t>Guidato</t>
+  </si>
+  <si>
+    <t>VIAGGIO</t>
+  </si>
+  <si>
+    <t>GIORNO</t>
+  </si>
+  <si>
+    <t>SETTIMANA</t>
+  </si>
+  <si>
+    <t>MESE</t>
+  </si>
+  <si>
+    <t>ANNO</t>
+  </si>
+  <si>
+    <t>ANNUALE</t>
+  </si>
+  <si>
+    <t>Período</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Información</t>
+  </si>
+  <si>
+    <t>Cuentakilómetros</t>
+  </si>
+  <si>
+    <t>mínimo</t>
+  </si>
+  <si>
+    <t>máx.</t>
+  </si>
+  <si>
+    <t>#cargando</t>
+  </si>
+  <si>
+    <t>#Excursiones</t>
+  </si>
+  <si>
+    <t>Alcance</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>actualización GPS</t>
+  </si>
+  <si>
+    <t>Última entrada</t>
+  </si>
+  <si>
+    <t>última dirección</t>
+  </si>
+  <si>
+    <t>Impulsado</t>
+  </si>
+  <si>
+    <t>VIAJE</t>
+  </si>
+  <si>
+    <t>DÍA</t>
+  </si>
+  <si>
+    <t>SEMANA</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>AÑO</t>
+  </si>
+  <si>
+    <t>PROMEDIO DÍA</t>
+  </si>
+  <si>
+    <t>ANUAL</t>
+  </si>
+  <si>
+    <t>Vägmätare</t>
+  </si>
+  <si>
+    <t>Kosta</t>
+  </si>
+  <si>
+    <t>#Laddning</t>
+  </si>
+  <si>
+    <t>#Resor</t>
+  </si>
+  <si>
+    <t>Räckvidd</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>GPS-uppdatering</t>
+  </si>
+  <si>
+    <t>Sista inlägget</t>
+  </si>
+  <si>
+    <t>Sista adressen</t>
+  </si>
+  <si>
+    <t>RESA</t>
+  </si>
+  <si>
+    <t>VECKA</t>
+  </si>
+  <si>
+    <t>MÅNAD</t>
+  </si>
+  <si>
+    <t>ÅR</t>
+  </si>
+  <si>
+    <t>ÅRLIG</t>
+  </si>
+  <si>
+    <t>TRIP AVG</t>
+  </si>
+  <si>
+    <t>DAY AVG</t>
+  </si>
+  <si>
+    <t>WEEK AVG</t>
+  </si>
+  <si>
+    <t>MONTH AVG</t>
+  </si>
+  <si>
+    <t>Dato</t>
+  </si>
+  <si>
+    <t>Kilometerteller</t>
+  </si>
+  <si>
+    <t>Koste</t>
+  </si>
+  <si>
+    <t>SOC %</t>
+  </si>
+  <si>
+    <t>Gj.sn</t>
+  </si>
+  <si>
+    <t>Maks</t>
+  </si>
+  <si>
+    <t>12V %</t>
+  </si>
+  <si>
+    <t>#Lading</t>
+  </si>
+  <si>
+    <t>#Turer</t>
+  </si>
+  <si>
+    <t>Område</t>
+  </si>
+  <si>
+    <t>Oppdatering av kjøretøy</t>
+  </si>
+  <si>
+    <t>GPS-oppdatering</t>
+  </si>
+  <si>
+    <t>Siste oppføring</t>
+  </si>
+  <si>
+    <t>Siste adresse</t>
+  </si>
+  <si>
+    <t>Kjørt</t>
+  </si>
+  <si>
+    <t>TUR</t>
+  </si>
+  <si>
+    <t>UKE</t>
+  </si>
+  <si>
+    <t>MÅNED</t>
+  </si>
+  <si>
+    <t>TUR GJENS</t>
+  </si>
+  <si>
+    <t>DAG GEN</t>
+  </si>
+  <si>
+    <t>UKE GJENSN</t>
+  </si>
+  <si>
+    <t>MÅNED GJENS</t>
+  </si>
+  <si>
+    <t>Uppdatering av fordon</t>
+  </si>
+  <si>
+    <t>RESA AVG</t>
+  </si>
+  <si>
+    <t>DAG AVG</t>
+  </si>
+  <si>
+    <t>VECKA AVG</t>
+  </si>
+  <si>
+    <t>MÅNAD AVG</t>
+  </si>
+  <si>
+    <t>Actualización del vehículo</t>
+  </si>
+  <si>
+    <t>VIAJE PROMEDIO</t>
+  </si>
+  <si>
+    <t>PROMEDIO DE LA SEMANA</t>
+  </si>
+  <si>
+    <t>PROMEDIO DEL MES</t>
+  </si>
+  <si>
+    <t>Aggiornamento del veicolo</t>
+  </si>
+  <si>
+    <t>MEDIA VIAGGIO</t>
+  </si>
+  <si>
+    <t>MEDIA GIORNO</t>
+  </si>
+  <si>
+    <t>MEDIA SETTIMANA</t>
+  </si>
+  <si>
+    <t>MEDIA MESE</t>
+  </si>
+  <si>
+    <t>MOYENNE VOYAGE</t>
+  </si>
+  <si>
+    <t>MOYENNE JOUR</t>
+  </si>
+  <si>
+    <t>MOYENNE DE LA SEMAINE</t>
+  </si>
+  <si>
+    <t>MOIS MOIS</t>
+  </si>
+  <si>
+    <t>Kilometertæller</t>
+  </si>
+  <si>
+    <t>Gns</t>
+  </si>
+  <si>
+    <t>#Opladning</t>
+  </si>
+  <si>
+    <t>#Rejser</t>
+  </si>
+  <si>
+    <t>Rækkevidde</t>
+  </si>
+  <si>
+    <t>Opdatering af køretøj</t>
+  </si>
+  <si>
+    <t>GPS opdatering</t>
+  </si>
+  <si>
+    <t>Sidste indgang</t>
+  </si>
+  <si>
+    <t>Sidste adresse</t>
+  </si>
+  <si>
+    <t>Kørt</t>
+  </si>
+  <si>
+    <t>REJSE</t>
+  </si>
+  <si>
+    <t>UGE</t>
+  </si>
+  <si>
+    <t>TRIP GEN</t>
+  </si>
+  <si>
+    <t>DAG GNS</t>
+  </si>
+  <si>
+    <t>UGE GNS</t>
+  </si>
+  <si>
+    <t>MÅNED GNS</t>
+  </si>
+  <si>
+    <t>ÅRLIGT</t>
+  </si>
+  <si>
+    <t>Kausi</t>
+  </si>
+  <si>
+    <t>Päivämäärä</t>
+  </si>
+  <si>
+    <t>Tiedot</t>
+  </si>
+  <si>
+    <t>Matkamittari</t>
+  </si>
+  <si>
+    <t>Kustannus</t>
+  </si>
+  <si>
+    <t>Keskim</t>
+  </si>
+  <si>
+    <t>12 V %</t>
+  </si>
+  <si>
+    <t>#Lataa</t>
+  </si>
+  <si>
+    <t>#Matkoja</t>
+  </si>
+  <si>
+    <t>Alue</t>
+  </si>
+  <si>
+    <t>Osoite</t>
+  </si>
+  <si>
+    <t>Ajoneuvon päivitys</t>
+  </si>
+  <si>
+    <t>GPS-päivitys</t>
+  </si>
+  <si>
+    <t>Viimeinen sisääntulo</t>
+  </si>
+  <si>
+    <t>Viimeinen osoite</t>
+  </si>
+  <si>
+    <t>Ajettu</t>
+  </si>
+  <si>
+    <t>MATKA</t>
+  </si>
+  <si>
+    <t>PÄIVÄ</t>
+  </si>
+  <si>
+    <t>VIIKKO</t>
+  </si>
+  <si>
+    <t>KUUKAUSI</t>
+  </si>
+  <si>
+    <t>VUOSI</t>
+  </si>
+  <si>
+    <t>PÄIVÄ AVG</t>
+  </si>
+  <si>
+    <t>VIIKKO KESK</t>
+  </si>
+  <si>
+    <t>KUUKAUDEN KESK</t>
+  </si>
+  <si>
+    <t>VUOSITTAIN</t>
+  </si>
+  <si>
+    <t>Encontro</t>
+  </si>
+  <si>
+    <t>Informações</t>
+  </si>
+  <si>
+    <t>hodômetro</t>
+  </si>
+  <si>
+    <t>Custo</t>
+  </si>
+  <si>
+    <t>médio</t>
+  </si>
+  <si>
+    <t>mín.</t>
+  </si>
+  <si>
+    <t>#Carregando</t>
+  </si>
+  <si>
+    <t>#viagens</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Atualização do veículo</t>
+  </si>
+  <si>
+    <t>atualização de GPS</t>
+  </si>
+  <si>
+    <t>último endereço</t>
+  </si>
+  <si>
+    <t>Dirigido</t>
+  </si>
+  <si>
+    <t>VIAGEM</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>MÊS</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>DIA AVG</t>
+  </si>
+  <si>
+    <t>SEMANA AVG</t>
+  </si>
+  <si>
+    <t>MÉD DO MÊS</t>
+  </si>
+  <si>
+    <t>gef.</t>
+  </si>
+  <si>
+    <t>FAHRT-Ø</t>
+  </si>
+  <si>
+    <t>TAG-Ø</t>
+  </si>
+  <si>
+    <t>WOCHE-Ø</t>
+  </si>
+  <si>
+    <t>MONATS-Ø</t>
+  </si>
+  <si>
+    <t>RIT-Ø</t>
+  </si>
+  <si>
+    <t>DAG-Ø</t>
+  </si>
+  <si>
+    <t>WEEK-Ø</t>
+  </si>
+  <si>
+    <t>MAAND-Ø</t>
+  </si>
+  <si>
+    <t>Batt.onderh.</t>
   </si>
 </sst>
 </file>
@@ -1081,18 +1870,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
@@ -1214,7 +2005,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
         <v>207</v>
@@ -1439,7 +2230,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
         <v>226</v>
@@ -1477,10 +2268,10 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
-        <v>231</v>
+        <v>497</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
@@ -1518,7 +2309,7 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>279</v>
       </c>
       <c r="D11" t="s">
         <v>198</v>
@@ -1591,10 +2382,10 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C13" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="D13" t="s">
         <v>208</v>
@@ -1984,6 +2775,1146 @@
       </c>
       <c r="C23" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" t="s">
+        <v>285</v>
+      </c>
+      <c r="E24" t="s">
+        <v>307</v>
+      </c>
+      <c r="F24" t="s">
+        <v>327</v>
+      </c>
+      <c r="G24" t="s">
+        <v>347</v>
+      </c>
+      <c r="H24" t="s">
+        <v>240</v>
+      </c>
+      <c r="I24" t="s">
+        <v>243</v>
+      </c>
+      <c r="J24" t="s">
+        <v>243</v>
+      </c>
+      <c r="K24" t="s">
+        <v>443</v>
+      </c>
+      <c r="L24" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>255</v>
+      </c>
+      <c r="B25" t="s">
+        <v>255</v>
+      </c>
+      <c r="C25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" t="s">
+        <v>286</v>
+      </c>
+      <c r="E25" t="s">
+        <v>255</v>
+      </c>
+      <c r="F25" t="s">
+        <v>328</v>
+      </c>
+      <c r="G25" t="s">
+        <v>348</v>
+      </c>
+      <c r="H25" t="s">
+        <v>286</v>
+      </c>
+      <c r="I25" t="s">
+        <v>386</v>
+      </c>
+      <c r="J25" t="s">
+        <v>386</v>
+      </c>
+      <c r="K25" t="s">
+        <v>444</v>
+      </c>
+      <c r="L25" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B26" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26" t="s">
+        <v>254</v>
+      </c>
+      <c r="E26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F26" t="s">
+        <v>329</v>
+      </c>
+      <c r="G26" t="s">
+        <v>349</v>
+      </c>
+      <c r="H26" t="s">
+        <v>254</v>
+      </c>
+      <c r="I26" t="s">
+        <v>254</v>
+      </c>
+      <c r="J26" t="s">
+        <v>254</v>
+      </c>
+      <c r="K26" t="s">
+        <v>445</v>
+      </c>
+      <c r="L26" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" t="s">
+        <v>253</v>
+      </c>
+      <c r="C27" t="s">
+        <v>282</v>
+      </c>
+      <c r="D27" t="s">
+        <v>287</v>
+      </c>
+      <c r="E27" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" t="s">
+        <v>330</v>
+      </c>
+      <c r="G27" t="s">
+        <v>350</v>
+      </c>
+      <c r="H27" t="s">
+        <v>368</v>
+      </c>
+      <c r="I27" t="s">
+        <v>387</v>
+      </c>
+      <c r="J27" t="s">
+        <v>426</v>
+      </c>
+      <c r="K27" t="s">
+        <v>446</v>
+      </c>
+      <c r="L27" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>252</v>
+      </c>
+      <c r="B28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" t="s">
+        <v>252</v>
+      </c>
+      <c r="D28" t="s">
+        <v>488</v>
+      </c>
+      <c r="E28" t="s">
+        <v>252</v>
+      </c>
+      <c r="F28" t="s">
+        <v>252</v>
+      </c>
+      <c r="G28" t="s">
+        <v>252</v>
+      </c>
+      <c r="H28" t="s">
+        <v>252</v>
+      </c>
+      <c r="I28" t="s">
+        <v>252</v>
+      </c>
+      <c r="J28" t="s">
+        <v>252</v>
+      </c>
+      <c r="K28" t="s">
+        <v>252</v>
+      </c>
+      <c r="L28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>251</v>
+      </c>
+      <c r="B29" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" t="s">
+        <v>278</v>
+      </c>
+      <c r="D29" t="s">
+        <v>278</v>
+      </c>
+      <c r="E29" t="s">
+        <v>309</v>
+      </c>
+      <c r="F29" t="s">
+        <v>331</v>
+      </c>
+      <c r="G29" t="s">
+        <v>331</v>
+      </c>
+      <c r="H29" t="s">
+        <v>369</v>
+      </c>
+      <c r="I29" t="s">
+        <v>388</v>
+      </c>
+      <c r="J29" t="s">
+        <v>388</v>
+      </c>
+      <c r="K29" t="s">
+        <v>447</v>
+      </c>
+      <c r="L29" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" t="s">
+        <v>241</v>
+      </c>
+      <c r="C30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" t="s">
+        <v>310</v>
+      </c>
+      <c r="F30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G30" t="s">
+        <v>241</v>
+      </c>
+      <c r="H30" t="s">
+        <v>241</v>
+      </c>
+      <c r="I30" t="s">
+        <v>389</v>
+      </c>
+      <c r="J30" t="s">
+        <v>389</v>
+      </c>
+      <c r="K30" t="s">
+        <v>389</v>
+      </c>
+      <c r="L30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C31" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" t="s">
+        <v>208</v>
+      </c>
+      <c r="E31" t="s">
+        <v>311</v>
+      </c>
+      <c r="F31" t="s">
+        <v>219</v>
+      </c>
+      <c r="G31" t="s">
+        <v>220</v>
+      </c>
+      <c r="H31" t="s">
+        <v>221</v>
+      </c>
+      <c r="I31" t="s">
+        <v>390</v>
+      </c>
+      <c r="J31" t="s">
+        <v>427</v>
+      </c>
+      <c r="K31" t="s">
+        <v>448</v>
+      </c>
+      <c r="L31" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B32" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D32" t="s">
+        <v>302</v>
+      </c>
+      <c r="E32" t="s">
+        <v>280</v>
+      </c>
+      <c r="F32" t="s">
+        <v>302</v>
+      </c>
+      <c r="G32" t="s">
+        <v>351</v>
+      </c>
+      <c r="H32" t="s">
+        <v>280</v>
+      </c>
+      <c r="I32" t="s">
+        <v>280</v>
+      </c>
+      <c r="J32" t="s">
+        <v>280</v>
+      </c>
+      <c r="K32" t="s">
+        <v>280</v>
+      </c>
+      <c r="L32" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>236</v>
+      </c>
+      <c r="B33" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" t="s">
+        <v>217</v>
+      </c>
+      <c r="D33" t="s">
+        <v>288</v>
+      </c>
+      <c r="E33" t="s">
+        <v>217</v>
+      </c>
+      <c r="F33" t="s">
+        <v>332</v>
+      </c>
+      <c r="G33" t="s">
+        <v>352</v>
+      </c>
+      <c r="H33" t="s">
+        <v>217</v>
+      </c>
+      <c r="I33" t="s">
+        <v>391</v>
+      </c>
+      <c r="J33" t="s">
+        <v>391</v>
+      </c>
+      <c r="K33" t="s">
+        <v>217</v>
+      </c>
+      <c r="L33" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>263</v>
+      </c>
+      <c r="B34" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D34" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" t="s">
+        <v>242</v>
+      </c>
+      <c r="F34" t="s">
+        <v>242</v>
+      </c>
+      <c r="G34" t="s">
+        <v>242</v>
+      </c>
+      <c r="H34" t="s">
+        <v>242</v>
+      </c>
+      <c r="I34" t="s">
+        <v>392</v>
+      </c>
+      <c r="J34" t="s">
+        <v>242</v>
+      </c>
+      <c r="K34" t="s">
+        <v>449</v>
+      </c>
+      <c r="L34" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>237</v>
+      </c>
+      <c r="B35" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D35" t="s">
+        <v>301</v>
+      </c>
+      <c r="E35" t="s">
+        <v>312</v>
+      </c>
+      <c r="F35" t="s">
+        <v>333</v>
+      </c>
+      <c r="G35" t="s">
+        <v>353</v>
+      </c>
+      <c r="H35" t="s">
+        <v>370</v>
+      </c>
+      <c r="I35" t="s">
+        <v>393</v>
+      </c>
+      <c r="J35" t="s">
+        <v>428</v>
+      </c>
+      <c r="K35" t="s">
+        <v>450</v>
+      </c>
+      <c r="L35" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>260</v>
+      </c>
+      <c r="B36" t="s">
+        <v>261</v>
+      </c>
+      <c r="C36" t="s">
+        <v>306</v>
+      </c>
+      <c r="D36" t="s">
+        <v>300</v>
+      </c>
+      <c r="E36" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" t="s">
+        <v>334</v>
+      </c>
+      <c r="G36" t="s">
+        <v>354</v>
+      </c>
+      <c r="H36" t="s">
+        <v>371</v>
+      </c>
+      <c r="I36" t="s">
+        <v>394</v>
+      </c>
+      <c r="J36" t="s">
+        <v>429</v>
+      </c>
+      <c r="K36" t="s">
+        <v>451</v>
+      </c>
+      <c r="L36" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" t="s">
+        <v>283</v>
+      </c>
+      <c r="C37" t="s">
+        <v>284</v>
+      </c>
+      <c r="D37" t="s">
+        <v>289</v>
+      </c>
+      <c r="E37" t="s">
+        <v>314</v>
+      </c>
+      <c r="F37" t="s">
+        <v>335</v>
+      </c>
+      <c r="G37" t="s">
+        <v>355</v>
+      </c>
+      <c r="H37" t="s">
+        <v>372</v>
+      </c>
+      <c r="I37" t="s">
+        <v>395</v>
+      </c>
+      <c r="J37" t="s">
+        <v>430</v>
+      </c>
+      <c r="K37" t="s">
+        <v>452</v>
+      </c>
+      <c r="L37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" t="s">
+        <v>245</v>
+      </c>
+      <c r="D38" t="s">
+        <v>315</v>
+      </c>
+      <c r="E38" t="s">
+        <v>315</v>
+      </c>
+      <c r="F38" t="s">
+        <v>336</v>
+      </c>
+      <c r="G38" t="s">
+        <v>356</v>
+      </c>
+      <c r="H38" t="s">
+        <v>373</v>
+      </c>
+      <c r="I38" t="s">
+        <v>315</v>
+      </c>
+      <c r="J38" t="s">
+        <v>315</v>
+      </c>
+      <c r="K38" t="s">
+        <v>453</v>
+      </c>
+      <c r="L38" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>246</v>
+      </c>
+      <c r="B39" t="s">
+        <v>246</v>
+      </c>
+      <c r="C39" t="s">
+        <v>256</v>
+      </c>
+      <c r="D39" t="s">
+        <v>290</v>
+      </c>
+      <c r="E39" t="s">
+        <v>316</v>
+      </c>
+      <c r="F39" t="s">
+        <v>417</v>
+      </c>
+      <c r="G39" t="s">
+        <v>413</v>
+      </c>
+      <c r="H39" t="s">
+        <v>408</v>
+      </c>
+      <c r="I39" t="s">
+        <v>396</v>
+      </c>
+      <c r="J39" t="s">
+        <v>431</v>
+      </c>
+      <c r="K39" t="s">
+        <v>454</v>
+      </c>
+      <c r="L39" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C40" t="s">
+        <v>247</v>
+      </c>
+      <c r="D40" t="s">
+        <v>291</v>
+      </c>
+      <c r="E40" t="s">
+        <v>317</v>
+      </c>
+      <c r="F40" t="s">
+        <v>337</v>
+      </c>
+      <c r="G40" t="s">
+        <v>357</v>
+      </c>
+      <c r="H40" t="s">
+        <v>374</v>
+      </c>
+      <c r="I40" t="s">
+        <v>397</v>
+      </c>
+      <c r="J40" t="s">
+        <v>432</v>
+      </c>
+      <c r="K40" t="s">
+        <v>455</v>
+      </c>
+      <c r="L40" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>248</v>
+      </c>
+      <c r="B41" t="s">
+        <v>248</v>
+      </c>
+      <c r="C41" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" t="s">
+        <v>292</v>
+      </c>
+      <c r="E41" t="s">
+        <v>318</v>
+      </c>
+      <c r="F41" t="s">
+        <v>338</v>
+      </c>
+      <c r="G41" t="s">
+        <v>358</v>
+      </c>
+      <c r="H41" t="s">
+        <v>375</v>
+      </c>
+      <c r="I41" t="s">
+        <v>398</v>
+      </c>
+      <c r="J41" t="s">
+        <v>433</v>
+      </c>
+      <c r="K41" t="s">
+        <v>456</v>
+      </c>
+      <c r="L41" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>249</v>
+      </c>
+      <c r="B42" t="s">
+        <v>249</v>
+      </c>
+      <c r="C42" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" t="s">
+        <v>293</v>
+      </c>
+      <c r="E42" t="s">
+        <v>319</v>
+      </c>
+      <c r="F42" t="s">
+        <v>339</v>
+      </c>
+      <c r="G42" t="s">
+        <v>359</v>
+      </c>
+      <c r="H42" t="s">
+        <v>376</v>
+      </c>
+      <c r="I42" t="s">
+        <v>399</v>
+      </c>
+      <c r="J42" t="s">
+        <v>434</v>
+      </c>
+      <c r="K42" t="s">
+        <v>457</v>
+      </c>
+      <c r="L42" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>250</v>
+      </c>
+      <c r="B43" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" t="s">
+        <v>294</v>
+      </c>
+      <c r="E43" t="s">
+        <v>320</v>
+      </c>
+      <c r="F43" t="s">
+        <v>340</v>
+      </c>
+      <c r="G43" t="s">
+        <v>360</v>
+      </c>
+      <c r="H43" t="s">
+        <v>250</v>
+      </c>
+      <c r="I43" t="s">
+        <v>400</v>
+      </c>
+      <c r="J43" t="s">
+        <v>435</v>
+      </c>
+      <c r="K43" t="s">
+        <v>458</v>
+      </c>
+      <c r="L43" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>264</v>
+      </c>
+      <c r="B44" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44" t="s">
+        <v>281</v>
+      </c>
+      <c r="D44" t="s">
+        <v>303</v>
+      </c>
+      <c r="E44" t="s">
+        <v>321</v>
+      </c>
+      <c r="F44" t="s">
+        <v>341</v>
+      </c>
+      <c r="G44" t="s">
+        <v>361</v>
+      </c>
+      <c r="H44" t="s">
+        <v>377</v>
+      </c>
+      <c r="I44" t="s">
+        <v>401</v>
+      </c>
+      <c r="J44" t="s">
+        <v>436</v>
+      </c>
+      <c r="K44" t="s">
+        <v>459</v>
+      </c>
+      <c r="L44" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" t="s">
+        <v>265</v>
+      </c>
+      <c r="C45" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" t="s">
+        <v>295</v>
+      </c>
+      <c r="E45" t="s">
+        <v>322</v>
+      </c>
+      <c r="F45" t="s">
+        <v>342</v>
+      </c>
+      <c r="G45" t="s">
+        <v>362</v>
+      </c>
+      <c r="H45" t="s">
+        <v>274</v>
+      </c>
+      <c r="I45" t="s">
+        <v>274</v>
+      </c>
+      <c r="J45" t="s">
+        <v>274</v>
+      </c>
+      <c r="K45" t="s">
+        <v>460</v>
+      </c>
+      <c r="L45" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" t="s">
+        <v>266</v>
+      </c>
+      <c r="B46" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46" t="s">
+        <v>266</v>
+      </c>
+      <c r="D46" t="s">
+        <v>296</v>
+      </c>
+      <c r="E46" t="s">
+        <v>323</v>
+      </c>
+      <c r="F46" t="s">
+        <v>343</v>
+      </c>
+      <c r="G46" t="s">
+        <v>363</v>
+      </c>
+      <c r="H46" t="s">
+        <v>378</v>
+      </c>
+      <c r="I46" t="s">
+        <v>402</v>
+      </c>
+      <c r="J46" t="s">
+        <v>437</v>
+      </c>
+      <c r="K46" t="s">
+        <v>461</v>
+      </c>
+      <c r="L46" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" t="s">
+        <v>267</v>
+      </c>
+      <c r="B47" t="s">
+        <v>267</v>
+      </c>
+      <c r="C47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D47" t="s">
+        <v>297</v>
+      </c>
+      <c r="E47" t="s">
+        <v>324</v>
+      </c>
+      <c r="F47" t="s">
+        <v>344</v>
+      </c>
+      <c r="G47" t="s">
+        <v>364</v>
+      </c>
+      <c r="H47" t="s">
+        <v>379</v>
+      </c>
+      <c r="I47" t="s">
+        <v>403</v>
+      </c>
+      <c r="J47" t="s">
+        <v>403</v>
+      </c>
+      <c r="K47" t="s">
+        <v>462</v>
+      </c>
+      <c r="L47" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" t="s">
+        <v>268</v>
+      </c>
+      <c r="B48" t="s">
+        <v>268</v>
+      </c>
+      <c r="C48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" t="s">
+        <v>298</v>
+      </c>
+      <c r="E48" t="s">
+        <v>325</v>
+      </c>
+      <c r="F48" t="s">
+        <v>345</v>
+      </c>
+      <c r="G48" t="s">
+        <v>365</v>
+      </c>
+      <c r="H48" t="s">
+        <v>380</v>
+      </c>
+      <c r="I48" t="s">
+        <v>380</v>
+      </c>
+      <c r="J48" t="s">
+        <v>380</v>
+      </c>
+      <c r="K48" t="s">
+        <v>463</v>
+      </c>
+      <c r="L48" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>269</v>
+      </c>
+      <c r="B49" t="s">
+        <v>382</v>
+      </c>
+      <c r="C49" t="s">
+        <v>493</v>
+      </c>
+      <c r="D49" t="s">
+        <v>489</v>
+      </c>
+      <c r="E49" t="s">
+        <v>422</v>
+      </c>
+      <c r="F49" t="s">
+        <v>418</v>
+      </c>
+      <c r="G49" t="s">
+        <v>414</v>
+      </c>
+      <c r="H49" t="s">
+        <v>409</v>
+      </c>
+      <c r="I49" t="s">
+        <v>404</v>
+      </c>
+      <c r="J49" t="s">
+        <v>438</v>
+      </c>
+      <c r="K49" t="s">
+        <v>382</v>
+      </c>
+      <c r="L49" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" t="s">
+        <v>383</v>
+      </c>
+      <c r="C50" t="s">
+        <v>494</v>
+      </c>
+      <c r="D50" t="s">
+        <v>490</v>
+      </c>
+      <c r="E50" t="s">
+        <v>423</v>
+      </c>
+      <c r="F50" t="s">
+        <v>419</v>
+      </c>
+      <c r="G50" t="s">
+        <v>366</v>
+      </c>
+      <c r="H50" t="s">
+        <v>410</v>
+      </c>
+      <c r="I50" t="s">
+        <v>405</v>
+      </c>
+      <c r="J50" t="s">
+        <v>439</v>
+      </c>
+      <c r="K50" t="s">
+        <v>464</v>
+      </c>
+      <c r="L50" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>271</v>
+      </c>
+      <c r="B51" t="s">
+        <v>384</v>
+      </c>
+      <c r="C51" t="s">
+        <v>495</v>
+      </c>
+      <c r="D51" t="s">
+        <v>491</v>
+      </c>
+      <c r="E51" t="s">
+        <v>424</v>
+      </c>
+      <c r="F51" t="s">
+        <v>420</v>
+      </c>
+      <c r="G51" t="s">
+        <v>415</v>
+      </c>
+      <c r="H51" t="s">
+        <v>411</v>
+      </c>
+      <c r="I51" t="s">
+        <v>406</v>
+      </c>
+      <c r="J51" t="s">
+        <v>440</v>
+      </c>
+      <c r="K51" t="s">
+        <v>465</v>
+      </c>
+      <c r="L51" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>272</v>
+      </c>
+      <c r="B52" t="s">
+        <v>385</v>
+      </c>
+      <c r="C52" t="s">
+        <v>496</v>
+      </c>
+      <c r="D52" t="s">
+        <v>492</v>
+      </c>
+      <c r="E52" t="s">
+        <v>425</v>
+      </c>
+      <c r="F52" t="s">
+        <v>421</v>
+      </c>
+      <c r="G52" t="s">
+        <v>416</v>
+      </c>
+      <c r="H52" t="s">
+        <v>412</v>
+      </c>
+      <c r="I52" t="s">
+        <v>407</v>
+      </c>
+      <c r="J52" t="s">
+        <v>441</v>
+      </c>
+      <c r="K52" t="s">
+        <v>466</v>
+      </c>
+      <c r="L52" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>273</v>
+      </c>
+      <c r="B53" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" t="s">
+        <v>277</v>
+      </c>
+      <c r="D53" t="s">
+        <v>299</v>
+      </c>
+      <c r="E53" t="s">
+        <v>326</v>
+      </c>
+      <c r="F53" t="s">
+        <v>346</v>
+      </c>
+      <c r="G53" t="s">
+        <v>367</v>
+      </c>
+      <c r="H53" t="s">
+        <v>381</v>
+      </c>
+      <c r="I53" t="s">
+        <v>381</v>
+      </c>
+      <c r="J53" t="s">
+        <v>442</v>
+      </c>
+      <c r="K53" t="s">
+        <v>467</v>
+      </c>
+      <c r="L53" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some Norwegian translations
</commit_message>
<xml_diff>
--- a/monitor.translations.xlsx
+++ b/monitor.translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick\git\monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA08C7A7-18EB-427C-9438-D037B722EE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A286E6A-8E00-4B6B-9A5A-C6871BDC6946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20445" yWindow="930" windowWidth="17805" windowHeight="18435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="22335" windowHeight="18435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="497">
   <si>
     <t>en</t>
   </si>
@@ -375,15 +375,9 @@
     <t>Dödtid</t>
   </si>
   <si>
-    <t>Siste løpetur</t>
-  </si>
-  <si>
     <t>Totaler</t>
   </si>
   <si>
-    <t>Restitusjon</t>
-  </si>
-  <si>
     <t>Forbruk</t>
   </si>
   <si>
@@ -396,9 +390,6 @@
     <t>Avstand</t>
   </si>
   <si>
-    <t>Inaktiv tid</t>
-  </si>
-  <si>
     <t>Sidste løbetur</t>
   </si>
   <si>
@@ -693,9 +684,6 @@
     <t>Genomsnittlig</t>
   </si>
   <si>
-    <t>Gj.sn.</t>
-  </si>
-  <si>
     <t>Gns.</t>
   </si>
   <si>
@@ -1197,9 +1185,6 @@
     <t>SOC %</t>
   </si>
   <si>
-    <t>Gj.sn</t>
-  </si>
-  <si>
     <t>Maks</t>
   </si>
   <si>
@@ -1239,18 +1224,6 @@
     <t>MÅNED</t>
   </si>
   <si>
-    <t>TUR GJENS</t>
-  </si>
-  <si>
-    <t>DAG GEN</t>
-  </si>
-  <si>
-    <t>UKE GJENSN</t>
-  </si>
-  <si>
-    <t>MÅNED GJENS</t>
-  </si>
-  <si>
     <t>Uppdatering av fordon</t>
   </si>
   <si>
@@ -1519,6 +1492,30 @@
   </si>
   <si>
     <t>Batt.onderh.</t>
+  </si>
+  <si>
+    <t>Siste tur</t>
+  </si>
+  <si>
+    <t>Gjenvinning</t>
+  </si>
+  <si>
+    <t>Snitt</t>
+  </si>
+  <si>
+    <t>Tomgang</t>
+  </si>
+  <si>
+    <t>TUR SNITT</t>
+  </si>
+  <si>
+    <t>DAG SNITT</t>
+  </si>
+  <si>
+    <t>UKE SNITT</t>
+  </si>
+  <si>
+    <t>MÅNED SNITT</t>
   </si>
 </sst>
 </file>
@@ -1873,10 +1870,10 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1899,7 +1896,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -2005,10 +2002,10 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E3" t="s">
         <v>77</v>
@@ -2023,16 +2020,16 @@
         <v>107</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>489</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -2046,7 +2043,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E4" t="s">
         <v>78</v>
@@ -2061,16 +2058,16 @@
         <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2084,7 +2081,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E5" t="s">
         <v>79</v>
@@ -2099,16 +2096,16 @@
         <v>109</v>
       </c>
       <c r="I5" t="s">
-        <v>118</v>
+        <v>490</v>
       </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -2137,13 +2134,13 @@
         <v>110</v>
       </c>
       <c r="I6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L6" t="s">
         <v>89</v>
@@ -2181,7 +2178,7 @@
         <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L7" t="s">
         <v>39</v>
@@ -2219,7 +2216,7 @@
         <v>48</v>
       </c>
       <c r="K8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L8" t="s">
         <v>91</v>
@@ -2230,37 +2227,37 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" t="s">
         <v>197</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" t="s">
+        <v>199</v>
+      </c>
+      <c r="H9" t="s">
         <v>200</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>201</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
+        <v>201</v>
+      </c>
+      <c r="K9" t="s">
         <v>202</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9" t="s">
         <v>203</v>
-      </c>
-      <c r="I9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J9" t="s">
-        <v>204</v>
-      </c>
-      <c r="K9" t="s">
-        <v>205</v>
-      </c>
-      <c r="L9" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2268,10 +2265,10 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
@@ -2289,16 +2286,16 @@
         <v>112</v>
       </c>
       <c r="I10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2309,10 +2306,10 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E11" t="s">
         <v>84</v>
@@ -2327,16 +2324,16 @@
         <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2350,7 +2347,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -2365,16 +2362,16 @@
         <v>114</v>
       </c>
       <c r="I12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
       </c>
       <c r="K12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2382,37 +2379,37 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E13" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" t="s">
         <v>218</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
+        <v>491</v>
+      </c>
+      <c r="J13" t="s">
         <v>219</v>
       </c>
-      <c r="G13" t="s">
+      <c r="K13" t="s">
         <v>220</v>
       </c>
-      <c r="H13" t="s">
+      <c r="L13" t="s">
         <v>221</v>
-      </c>
-      <c r="I13" t="s">
-        <v>222</v>
-      </c>
-      <c r="J13" t="s">
-        <v>223</v>
-      </c>
-      <c r="K13" t="s">
-        <v>224</v>
-      </c>
-      <c r="L13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2420,37 +2417,37 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" t="s">
         <v>210</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>211</v>
       </c>
-      <c r="G14" t="s">
+      <c r="J14" t="s">
         <v>212</v>
       </c>
-      <c r="H14" t="s">
-        <v>213</v>
-      </c>
-      <c r="I14" t="s">
-        <v>214</v>
-      </c>
-      <c r="J14" t="s">
-        <v>215</v>
-      </c>
       <c r="K14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L14" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2458,10 +2455,10 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D15" t="s">
         <v>50</v>
@@ -2479,16 +2476,16 @@
         <v>115</v>
       </c>
       <c r="I15" t="s">
-        <v>123</v>
+        <v>492</v>
       </c>
       <c r="J15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2505,7 +2502,7 @@
         <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F16" t="s">
         <v>70</v>
@@ -2514,19 +2511,19 @@
         <v>103</v>
       </c>
       <c r="H16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2543,7 +2540,7 @@
         <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F17" t="s">
         <v>72</v>
@@ -2552,19 +2549,19 @@
         <v>104</v>
       </c>
       <c r="H17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I17" t="s">
+        <v>149</v>
+      </c>
+      <c r="J17" t="s">
         <v>152</v>
       </c>
-      <c r="J17" t="s">
-        <v>155</v>
-      </c>
       <c r="K17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N17" s="3"/>
     </row>
@@ -2576,34 +2573,34 @@
         <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
         <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -2616,13 +2613,13 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
         <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F19" t="s">
         <v>74</v>
@@ -2631,19 +2628,19 @@
         <v>105</v>
       </c>
       <c r="H19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -2657,13 +2654,13 @@
         <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F20" t="s">
         <v>71</v>
@@ -2672,19 +2669,19 @@
         <v>106</v>
       </c>
       <c r="H20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N20" s="3"/>
     </row>
@@ -2696,7 +2693,7 @@
         <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
@@ -2708,22 +2705,22 @@
         <v>75</v>
       </c>
       <c r="G21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J21" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N21" s="3"/>
     </row>
@@ -2735,7 +2732,7 @@
         <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
         <v>69</v>
@@ -2747,1174 +2744,1174 @@
         <v>76</v>
       </c>
       <c r="G22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K22" t="s">
         <v>65</v>
       </c>
       <c r="L22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" t="s">
         <v>191</v>
-      </c>
-      <c r="C23" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C24" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E24" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F24" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G24" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="H24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I24" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J24" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="K24" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="L24" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E25" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F25" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G25" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="H25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I25" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="J25" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="K25" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="L25" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F26" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G26" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="H26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="J26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="K26" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="L26" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C27" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D27" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E27" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F27" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G27" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H27" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I27" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="J27" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="K27" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="L27" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D28" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="E28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="K28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="L28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B29" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C29" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D29" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E29" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H29" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="I29" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="J29" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="K29" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="L29" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E30" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I30" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="J30" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="K30" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="L30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E31" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G31" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I31" t="s">
-        <v>390</v>
+        <v>491</v>
       </c>
       <c r="J31" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="K31" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="L31" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D32" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F32" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G32" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="H32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K32" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L32" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D33" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F33" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G33" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I33" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="J33" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="K33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L33" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I34" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="J34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="K34" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="L34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B35" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C35" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D35" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E35" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F35" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G35" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H35" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I35" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="J35" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="K35" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="L35" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B36" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C36" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D36" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E36" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F36" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G36" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H36" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="I36" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="J36" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K36" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="L36" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C37" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D37" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E37" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F37" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G37" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H37" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I37" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="J37" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="K37" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="L37" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D38" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E38" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F38" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G38" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H38" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="I38" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J38" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K38" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="L38" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C39" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D39" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E39" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F39" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="G39" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="H39" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="I39" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="J39" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K39" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="L39" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D40" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E40" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F40" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G40" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="H40" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I40" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="J40" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="K40" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="L40" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B41" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D41" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E41" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F41" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G41" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H41" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I41" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="J41" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="K41" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="L41" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B42" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C42" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D42" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E42" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F42" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G42" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H42" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I42" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="J42" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="K42" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="L42" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B43" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C43" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D43" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E43" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F43" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G43" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H43" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I43" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="J43" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="K43" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="L43" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B44" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C44" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D44" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E44" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F44" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G44" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H44" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="I44" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="J44" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="K44" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="L44" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B45" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D45" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E45" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F45" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G45" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="I45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K45" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="L45" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B46" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C46" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D46" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E46" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F46" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G46" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H46" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I46" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="J46" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="K46" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="L46" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B47" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C47" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D47" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E47" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F47" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G47" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H47" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="I47" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="J47" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K47" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="L47" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C48" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D48" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E48" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F48" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G48" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H48" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="I48" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J48" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="K48" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="L48" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C49" t="s">
+        <v>484</v>
+      </c>
+      <c r="D49" t="s">
+        <v>480</v>
+      </c>
+      <c r="E49" t="s">
+        <v>413</v>
+      </c>
+      <c r="F49" t="s">
+        <v>409</v>
+      </c>
+      <c r="G49" t="s">
+        <v>405</v>
+      </c>
+      <c r="H49" t="s">
+        <v>400</v>
+      </c>
+      <c r="I49" t="s">
         <v>493</v>
       </c>
-      <c r="D49" t="s">
-        <v>489</v>
-      </c>
-      <c r="E49" t="s">
-        <v>422</v>
-      </c>
-      <c r="F49" t="s">
-        <v>418</v>
-      </c>
-      <c r="G49" t="s">
-        <v>414</v>
-      </c>
-      <c r="H49" t="s">
-        <v>409</v>
-      </c>
-      <c r="I49" t="s">
-        <v>404</v>
-      </c>
       <c r="J49" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="K49" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="L49" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B50" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C50" t="s">
+        <v>485</v>
+      </c>
+      <c r="D50" t="s">
+        <v>481</v>
+      </c>
+      <c r="E50" t="s">
+        <v>414</v>
+      </c>
+      <c r="F50" t="s">
+        <v>410</v>
+      </c>
+      <c r="G50" t="s">
+        <v>362</v>
+      </c>
+      <c r="H50" t="s">
+        <v>401</v>
+      </c>
+      <c r="I50" t="s">
         <v>494</v>
       </c>
-      <c r="D50" t="s">
-        <v>490</v>
-      </c>
-      <c r="E50" t="s">
-        <v>423</v>
-      </c>
-      <c r="F50" t="s">
-        <v>419</v>
-      </c>
-      <c r="G50" t="s">
-        <v>366</v>
-      </c>
-      <c r="H50" t="s">
-        <v>410</v>
-      </c>
-      <c r="I50" t="s">
-        <v>405</v>
-      </c>
       <c r="J50" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="K50" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="L50" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B51" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C51" t="s">
+        <v>486</v>
+      </c>
+      <c r="D51" t="s">
+        <v>482</v>
+      </c>
+      <c r="E51" t="s">
+        <v>415</v>
+      </c>
+      <c r="F51" t="s">
+        <v>411</v>
+      </c>
+      <c r="G51" t="s">
+        <v>406</v>
+      </c>
+      <c r="H51" t="s">
+        <v>402</v>
+      </c>
+      <c r="I51" t="s">
         <v>495</v>
       </c>
-      <c r="D51" t="s">
-        <v>491</v>
-      </c>
-      <c r="E51" t="s">
-        <v>424</v>
-      </c>
-      <c r="F51" t="s">
-        <v>420</v>
-      </c>
-      <c r="G51" t="s">
-        <v>415</v>
-      </c>
-      <c r="H51" t="s">
-        <v>411</v>
-      </c>
-      <c r="I51" t="s">
-        <v>406</v>
-      </c>
       <c r="J51" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="K51" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="L51" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B52" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C52" t="s">
+        <v>487</v>
+      </c>
+      <c r="D52" t="s">
+        <v>483</v>
+      </c>
+      <c r="E52" t="s">
+        <v>416</v>
+      </c>
+      <c r="F52" t="s">
+        <v>412</v>
+      </c>
+      <c r="G52" t="s">
+        <v>407</v>
+      </c>
+      <c r="H52" t="s">
+        <v>403</v>
+      </c>
+      <c r="I52" t="s">
         <v>496</v>
       </c>
-      <c r="D52" t="s">
-        <v>492</v>
-      </c>
-      <c r="E52" t="s">
-        <v>425</v>
-      </c>
-      <c r="F52" t="s">
-        <v>421</v>
-      </c>
-      <c r="G52" t="s">
-        <v>416</v>
-      </c>
-      <c r="H52" t="s">
-        <v>412</v>
-      </c>
-      <c r="I52" t="s">
-        <v>407</v>
-      </c>
       <c r="J52" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="K52" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="L52" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
+        <v>269</v>
+      </c>
+      <c r="B53" t="s">
+        <v>269</v>
+      </c>
+      <c r="C53" t="s">
         <v>273</v>
       </c>
-      <c r="B53" t="s">
-        <v>273</v>
-      </c>
-      <c r="C53" t="s">
-        <v>277</v>
-      </c>
       <c r="D53" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E53" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F53" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G53" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H53" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="I53" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="J53" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="K53" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="L53" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>